<commit_message>
Role integration in Leads page and fixes
</commit_message>
<xml_diff>
--- a/public/csv_template/excel_leads_template.xlsx
+++ b/public/csv_template/excel_leads_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADITYA\OneDrive\Documents\CRM_IQOL\IQOLCRM-frontend\public\csv_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADITYA\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52DB6167-EADE-4B16-8499-EAFE748199B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4A04D3-1361-45CC-ACD8-D59288DE23E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{10B43098-1B18-476B-BDD1-67628B74BD80}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,7 +413,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{53ECA0A7-E078-4997-942A-3E013C9BEADC}">
-      <formula1>"whatsapp campaign, whatsapp group, instagram, facebook, classified, organic, referral"</formula1>
+      <formula1>"whatsapp campaign, whatsapp group, meta, instagram, facebook, classified, organic, referral"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>